<commit_message>
change template for import of products in StockMovements
</commit_message>
<xml_diff>
--- a/public/Products import.xlsx
+++ b/public/Products import.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27321"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin1c\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sancha/Documents/WAPI/Wapi/Работа/Переход на 1С/UI/Инбаунды/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63A52F6-3A49-41C7-9FF4-339E51AE19ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4E1929-32AC-7948-B21B-4965AAAD5700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27240" windowHeight="16515" xr2:uid="{982C8F82-BBA0-A446-9013-4BF7A2E977B9}"/>
+    <workbookView xWindow="2520" yWindow="4280" windowWidth="26040" windowHeight="14940" xr2:uid="{982C8F82-BBA0-A446-9013-4BF7A2E977B9}"/>
   </bookViews>
   <sheets>
     <sheet name="TO BE FILLED" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -53,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -468,20 +479,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B3FFAD-4D1E-CB48-9FDD-688D8553F3C2}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.875" style="8"/>
     <col min="5" max="5" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -497,3494 +506,3494 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="4"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
+    <row r="47" spans="1:5">
+      <c r="A47" s="4"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="4"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
+    <row r="48" spans="1:5">
+      <c r="A48" s="4"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="4"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+    <row r="54" spans="1:5">
+      <c r="A54" s="4"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="4"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="4"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
+    <row r="56" spans="1:5">
+      <c r="A56" s="4"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
+    <row r="58" spans="1:5">
+      <c r="A58" s="4"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="4"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="4"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="4"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="4"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
+    <row r="62" spans="1:5">
+      <c r="A62" s="4"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="4"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="4"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="4"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
+    <row r="65" spans="1:5">
+      <c r="A65" s="4"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
+    <row r="66" spans="1:5">
+      <c r="A66" s="4"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="4"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
+    <row r="67" spans="1:5">
+      <c r="A67" s="4"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="4"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
+    <row r="68" spans="1:5">
+      <c r="A68" s="4"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="4"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
+    <row r="69" spans="1:5">
+      <c r="A69" s="4"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="4"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
+    <row r="70" spans="1:5">
+      <c r="A70" s="4"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="4"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
+    <row r="71" spans="1:5">
+      <c r="A71" s="4"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="4"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
+    <row r="72" spans="1:5">
+      <c r="A72" s="4"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="4"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
+    <row r="73" spans="1:5">
+      <c r="A73" s="4"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="4"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
+    <row r="74" spans="1:5">
+      <c r="A74" s="4"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="4"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
+    <row r="75" spans="1:5">
+      <c r="A75" s="4"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="4"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
+    <row r="76" spans="1:5">
+      <c r="A76" s="4"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
+    <row r="77" spans="1:5">
+      <c r="A77" s="4"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="4"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="7"/>
+    <row r="78" spans="1:5">
+      <c r="A78" s="4"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="4"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="7"/>
+    <row r="79" spans="1:5">
+      <c r="A79" s="4"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="4"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="7"/>
+    <row r="80" spans="1:5">
+      <c r="A80" s="4"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="4"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
+    <row r="81" spans="1:5">
+      <c r="A81" s="4"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="4"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
+    <row r="82" spans="1:5">
+      <c r="A82" s="4"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="4"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
+    <row r="83" spans="1:5">
+      <c r="A83" s="4"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="4"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="7"/>
+    <row r="84" spans="1:5">
+      <c r="A84" s="4"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="4"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
+    <row r="85" spans="1:5">
+      <c r="A85" s="4"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="4"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="7"/>
+    <row r="86" spans="1:5">
+      <c r="A86" s="4"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="4"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
+    <row r="87" spans="1:5">
+      <c r="A87" s="4"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="4"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="7"/>
+    <row r="88" spans="1:5">
+      <c r="A88" s="4"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="4"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="7"/>
+    <row r="89" spans="1:5">
+      <c r="A89" s="4"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="7"/>
+    <row r="90" spans="1:5">
+      <c r="A90" s="4"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="4"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="7"/>
+    <row r="91" spans="1:5">
+      <c r="A91" s="4"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="4"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="7"/>
+    <row r="92" spans="1:5">
+      <c r="A92" s="4"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
       <c r="E92" s="4"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
+    <row r="93" spans="1:5">
+      <c r="A93" s="4"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
       <c r="E93" s="4"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="7"/>
+    <row r="94" spans="1:5">
+      <c r="A94" s="4"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
       <c r="E94" s="4"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="7"/>
+    <row r="95" spans="1:5">
+      <c r="A95" s="4"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="4"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="7"/>
+    <row r="96" spans="1:5">
+      <c r="A96" s="4"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
       <c r="E96" s="4"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="7"/>
+    <row r="97" spans="1:5">
+      <c r="A97" s="4"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="7"/>
+    <row r="98" spans="1:5">
+      <c r="A98" s="4"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="4"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="7"/>
+    <row r="99" spans="1:5">
+      <c r="A99" s="4"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="7"/>
+    <row r="100" spans="1:5">
+      <c r="A100" s="4"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="7"/>
+    <row r="101" spans="1:5">
+      <c r="A101" s="4"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
       <c r="E101" s="4"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="7"/>
+    <row r="102" spans="1:5">
+      <c r="A102" s="4"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="4"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="7"/>
+    <row r="103" spans="1:5">
+      <c r="A103" s="4"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="4"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="7"/>
+    <row r="104" spans="1:5">
+      <c r="A104" s="4"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="4"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="7"/>
+    <row r="105" spans="1:5">
+      <c r="A105" s="4"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="4"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="7"/>
+    <row r="106" spans="1:5">
+      <c r="A106" s="4"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="4"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="7"/>
+    <row r="107" spans="1:5">
+      <c r="A107" s="4"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="4"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="7"/>
+    <row r="108" spans="1:5">
+      <c r="A108" s="4"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="4"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
+    <row r="109" spans="1:5">
+      <c r="A109" s="4"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
+    <row r="110" spans="1:5">
+      <c r="A110" s="4"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="4"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
+    <row r="111" spans="1:5">
+      <c r="A111" s="4"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="4"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="7"/>
+    <row r="112" spans="1:5">
+      <c r="A112" s="4"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="4"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="7"/>
+    <row r="113" spans="1:5">
+      <c r="A113" s="4"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="4"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="7"/>
+    <row r="114" spans="1:5">
+      <c r="A114" s="4"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="4"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="7"/>
+    <row r="115" spans="1:5">
+      <c r="A115" s="4"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="4"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="7"/>
+    <row r="116" spans="1:5">
+      <c r="A116" s="4"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="4"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="7"/>
+    <row r="117" spans="1:5">
+      <c r="A117" s="4"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="4"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="7"/>
+    <row r="118" spans="1:5">
+      <c r="A118" s="4"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="4"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="7"/>
+    <row r="119" spans="1:5">
+      <c r="A119" s="4"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="4"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="7"/>
+    <row r="120" spans="1:5">
+      <c r="A120" s="4"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="4"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="7"/>
+    <row r="121" spans="1:5">
+      <c r="A121" s="4"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="4"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="7"/>
+    <row r="122" spans="1:5">
+      <c r="A122" s="4"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="4"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="7"/>
+    <row r="123" spans="1:5">
+      <c r="A123" s="4"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="4"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="7"/>
+    <row r="124" spans="1:5">
+      <c r="A124" s="4"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="4"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="7"/>
+    <row r="125" spans="1:5">
+      <c r="A125" s="4"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="4"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="7"/>
+    <row r="126" spans="1:5">
+      <c r="A126" s="4"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="7"/>
+    <row r="127" spans="1:5">
+      <c r="A127" s="4"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="4"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="7"/>
+    <row r="128" spans="1:5">
+      <c r="A128" s="4"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="4"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="7"/>
+    <row r="129" spans="1:5">
+      <c r="A129" s="4"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
       <c r="E129" s="4"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="7"/>
+    <row r="130" spans="1:5">
+      <c r="A130" s="4"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
       <c r="E130" s="4"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="7"/>
+    <row r="131" spans="1:5">
+      <c r="A131" s="4"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="7"/>
+    <row r="132" spans="1:5">
+      <c r="A132" s="4"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="4"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="7"/>
+    <row r="133" spans="1:5">
+      <c r="A133" s="4"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="4"/>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="7"/>
+    <row r="134" spans="1:5">
+      <c r="A134" s="4"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
       <c r="E134" s="4"/>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="7"/>
+    <row r="135" spans="1:5">
+      <c r="A135" s="4"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="7"/>
+    <row r="136" spans="1:5">
+      <c r="A136" s="4"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
       <c r="E136" s="4"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="7"/>
+    <row r="137" spans="1:5">
+      <c r="A137" s="4"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
       <c r="E137" s="4"/>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="7"/>
+    <row r="138" spans="1:5">
+      <c r="A138" s="4"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="4"/>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="7"/>
+    <row r="139" spans="1:5">
+      <c r="A139" s="4"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="4"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="7"/>
+    <row r="140" spans="1:5">
+      <c r="A140" s="4"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
       <c r="E140" s="4"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="7"/>
+    <row r="141" spans="1:5">
+      <c r="A141" s="4"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
       <c r="E141" s="4"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" s="7"/>
+    <row r="142" spans="1:5">
+      <c r="A142" s="4"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
       <c r="E142" s="4"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="7"/>
+    <row r="143" spans="1:5">
+      <c r="A143" s="4"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="4"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" s="7"/>
+    <row r="144" spans="1:5">
+      <c r="A144" s="4"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
       <c r="E144" s="4"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="7"/>
+    <row r="145" spans="1:5">
+      <c r="A145" s="4"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
       <c r="E145" s="4"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" s="7"/>
+    <row r="146" spans="1:5">
+      <c r="A146" s="4"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
       <c r="E146" s="4"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="7"/>
+    <row r="147" spans="1:5">
+      <c r="A147" s="4"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
       <c r="E147" s="4"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="7"/>
+    <row r="148" spans="1:5">
+      <c r="A148" s="4"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
       <c r="E148" s="4"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="7"/>
+    <row r="149" spans="1:5">
+      <c r="A149" s="4"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
       <c r="E149" s="4"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="7"/>
+    <row r="150" spans="1:5">
+      <c r="A150" s="4"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
       <c r="E150" s="4"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="7"/>
+    <row r="151" spans="1:5">
+      <c r="A151" s="4"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
       <c r="E151" s="4"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="7"/>
+    <row r="152" spans="1:5">
+      <c r="A152" s="4"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
       <c r="E152" s="4"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="7"/>
+    <row r="153" spans="1:5">
+      <c r="A153" s="4"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="4"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="7"/>
+    <row r="154" spans="1:5">
+      <c r="A154" s="4"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="4"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="7"/>
+    <row r="155" spans="1:5">
+      <c r="A155" s="4"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
       <c r="E155" s="4"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="7"/>
+    <row r="156" spans="1:5">
+      <c r="A156" s="4"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
       <c r="E156" s="4"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" s="7"/>
+    <row r="157" spans="1:5">
+      <c r="A157" s="4"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
       <c r="E157" s="4"/>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" s="7"/>
+    <row r="158" spans="1:5">
+      <c r="A158" s="4"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
       <c r="E158" s="4"/>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="7"/>
+    <row r="159" spans="1:5">
+      <c r="A159" s="4"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
       <c r="E159" s="4"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="7"/>
+    <row r="160" spans="1:5">
+      <c r="A160" s="4"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
       <c r="E160" s="4"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="7"/>
+    <row r="161" spans="1:5">
+      <c r="A161" s="4"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="4"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="7"/>
+    <row r="162" spans="1:5">
+      <c r="A162" s="4"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
       <c r="E162" s="4"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="7"/>
+    <row r="163" spans="1:5">
+      <c r="A163" s="4"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
       <c r="E163" s="4"/>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="7"/>
+    <row r="164" spans="1:5">
+      <c r="A164" s="4"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="4"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="7"/>
+    <row r="165" spans="1:5">
+      <c r="A165" s="4"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
       <c r="E165" s="4"/>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="7"/>
+    <row r="166" spans="1:5">
+      <c r="A166" s="4"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="4"/>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="7"/>
+    <row r="167" spans="1:5">
+      <c r="A167" s="4"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
       <c r="E167" s="4"/>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="7"/>
+    <row r="168" spans="1:5">
+      <c r="A168" s="4"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
       <c r="E168" s="4"/>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="7"/>
+    <row r="169" spans="1:5">
+      <c r="A169" s="4"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
       <c r="D169" s="7"/>
       <c r="E169" s="4"/>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="7"/>
+    <row r="170" spans="1:5">
+      <c r="A170" s="4"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
       <c r="E170" s="4"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="7"/>
+    <row r="171" spans="1:5">
+      <c r="A171" s="4"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
       <c r="E171" s="4"/>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="7"/>
+    <row r="172" spans="1:5">
+      <c r="A172" s="4"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="4"/>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="7"/>
+    <row r="173" spans="1:5">
+      <c r="A173" s="4"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
       <c r="D173" s="7"/>
       <c r="E173" s="4"/>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="7"/>
+    <row r="174" spans="1:5">
+      <c r="A174" s="4"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
       <c r="E174" s="4"/>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="7"/>
+    <row r="175" spans="1:5">
+      <c r="A175" s="4"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
       <c r="D175" s="7"/>
       <c r="E175" s="4"/>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="7"/>
+    <row r="176" spans="1:5">
+      <c r="A176" s="4"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
       <c r="D176" s="7"/>
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="7"/>
+    <row r="177" spans="1:5">
+      <c r="A177" s="4"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
       <c r="D177" s="7"/>
       <c r="E177" s="4"/>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="7"/>
+    <row r="178" spans="1:5">
+      <c r="A178" s="4"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
       <c r="D178" s="7"/>
       <c r="E178" s="4"/>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="7"/>
+    <row r="179" spans="1:5">
+      <c r="A179" s="4"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
       <c r="D179" s="7"/>
       <c r="E179" s="4"/>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="7"/>
+    <row r="180" spans="1:5">
+      <c r="A180" s="4"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
       <c r="D180" s="7"/>
       <c r="E180" s="4"/>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" s="7"/>
+    <row r="181" spans="1:5">
+      <c r="A181" s="4"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
       <c r="D181" s="7"/>
       <c r="E181" s="4"/>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" s="7"/>
+    <row r="182" spans="1:5">
+      <c r="A182" s="4"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
       <c r="D182" s="7"/>
       <c r="E182" s="4"/>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="7"/>
+    <row r="183" spans="1:5">
+      <c r="A183" s="4"/>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
       <c r="D183" s="7"/>
       <c r="E183" s="4"/>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" s="7"/>
+    <row r="184" spans="1:5">
+      <c r="A184" s="4"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
       <c r="D184" s="7"/>
       <c r="E184" s="4"/>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" s="7"/>
+    <row r="185" spans="1:5">
+      <c r="A185" s="4"/>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
       <c r="D185" s="7"/>
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" s="7"/>
+    <row r="186" spans="1:5">
+      <c r="A186" s="4"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
       <c r="D186" s="7"/>
       <c r="E186" s="4"/>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" s="7"/>
+    <row r="187" spans="1:5">
+      <c r="A187" s="4"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
       <c r="D187" s="7"/>
       <c r="E187" s="4"/>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="7"/>
+    <row r="188" spans="1:5">
+      <c r="A188" s="4"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
       <c r="D188" s="7"/>
       <c r="E188" s="4"/>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="7"/>
+    <row r="189" spans="1:5">
+      <c r="A189" s="4"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
       <c r="D189" s="7"/>
       <c r="E189" s="4"/>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="7"/>
+    <row r="190" spans="1:5">
+      <c r="A190" s="4"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
       <c r="D190" s="7"/>
       <c r="E190" s="4"/>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="7"/>
+    <row r="191" spans="1:5">
+      <c r="A191" s="4"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
       <c r="D191" s="7"/>
       <c r="E191" s="4"/>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="7"/>
+    <row r="192" spans="1:5">
+      <c r="A192" s="4"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
       <c r="D192" s="7"/>
       <c r="E192" s="4"/>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" s="7"/>
+    <row r="193" spans="1:5">
+      <c r="A193" s="4"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
       <c r="D193" s="7"/>
       <c r="E193" s="4"/>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" s="7"/>
+    <row r="194" spans="1:5">
+      <c r="A194" s="4"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
       <c r="D194" s="7"/>
       <c r="E194" s="4"/>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" s="7"/>
+    <row r="195" spans="1:5">
+      <c r="A195" s="4"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
       <c r="D195" s="7"/>
       <c r="E195" s="4"/>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" s="7"/>
+    <row r="196" spans="1:5">
+      <c r="A196" s="4"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
       <c r="D196" s="7"/>
       <c r="E196" s="4"/>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" s="7"/>
+    <row r="197" spans="1:5">
+      <c r="A197" s="4"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
       <c r="E197" s="4"/>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="7"/>
+    <row r="198" spans="1:5">
+      <c r="A198" s="4"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
       <c r="D198" s="7"/>
       <c r="E198" s="4"/>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="7"/>
+    <row r="199" spans="1:5">
+      <c r="A199" s="4"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
       <c r="D199" s="7"/>
       <c r="E199" s="4"/>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" s="7"/>
+    <row r="200" spans="1:5">
+      <c r="A200" s="4"/>
       <c r="B200" s="7"/>
       <c r="C200" s="7"/>
       <c r="D200" s="7"/>
       <c r="E200" s="4"/>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="7"/>
+    <row r="201" spans="1:5">
+      <c r="A201" s="4"/>
       <c r="B201" s="7"/>
       <c r="C201" s="7"/>
       <c r="D201" s="7"/>
       <c r="E201" s="4"/>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" s="7"/>
+    <row r="202" spans="1:5">
+      <c r="A202" s="4"/>
       <c r="B202" s="7"/>
       <c r="C202" s="7"/>
       <c r="D202" s="7"/>
       <c r="E202" s="4"/>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" s="7"/>
+    <row r="203" spans="1:5">
+      <c r="A203" s="4"/>
       <c r="B203" s="7"/>
       <c r="C203" s="7"/>
       <c r="D203" s="7"/>
       <c r="E203" s="4"/>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" s="7"/>
+    <row r="204" spans="1:5">
+      <c r="A204" s="4"/>
       <c r="B204" s="7"/>
       <c r="C204" s="7"/>
       <c r="D204" s="7"/>
       <c r="E204" s="4"/>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" s="7"/>
+    <row r="205" spans="1:5">
+      <c r="A205" s="4"/>
       <c r="B205" s="7"/>
       <c r="C205" s="7"/>
       <c r="D205" s="7"/>
       <c r="E205" s="4"/>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" s="7"/>
+    <row r="206" spans="1:5">
+      <c r="A206" s="4"/>
       <c r="B206" s="7"/>
       <c r="C206" s="7"/>
       <c r="D206" s="7"/>
       <c r="E206" s="4"/>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" s="7"/>
+    <row r="207" spans="1:5">
+      <c r="A207" s="4"/>
       <c r="B207" s="7"/>
       <c r="C207" s="7"/>
       <c r="D207" s="7"/>
       <c r="E207" s="4"/>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A208" s="7"/>
+    <row r="208" spans="1:5">
+      <c r="A208" s="4"/>
       <c r="B208" s="7"/>
       <c r="C208" s="7"/>
       <c r="D208" s="7"/>
       <c r="E208" s="4"/>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" s="7"/>
+    <row r="209" spans="1:5">
+      <c r="A209" s="4"/>
       <c r="B209" s="7"/>
       <c r="C209" s="7"/>
       <c r="D209" s="7"/>
       <c r="E209" s="4"/>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A210" s="7"/>
+    <row r="210" spans="1:5">
+      <c r="A210" s="4"/>
       <c r="B210" s="7"/>
       <c r="C210" s="7"/>
       <c r="D210" s="7"/>
       <c r="E210" s="4"/>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" s="7"/>
+    <row r="211" spans="1:5">
+      <c r="A211" s="4"/>
       <c r="B211" s="7"/>
       <c r="C211" s="7"/>
       <c r="D211" s="7"/>
       <c r="E211" s="4"/>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A212" s="7"/>
+    <row r="212" spans="1:5">
+      <c r="A212" s="4"/>
       <c r="B212" s="7"/>
       <c r="C212" s="7"/>
       <c r="D212" s="7"/>
       <c r="E212" s="4"/>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A213" s="7"/>
+    <row r="213" spans="1:5">
+      <c r="A213" s="4"/>
       <c r="B213" s="7"/>
       <c r="C213" s="7"/>
       <c r="D213" s="7"/>
       <c r="E213" s="4"/>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214" s="7"/>
+    <row r="214" spans="1:5">
+      <c r="A214" s="4"/>
       <c r="B214" s="7"/>
       <c r="C214" s="7"/>
       <c r="D214" s="7"/>
       <c r="E214" s="4"/>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" s="7"/>
+    <row r="215" spans="1:5">
+      <c r="A215" s="4"/>
       <c r="B215" s="7"/>
       <c r="C215" s="7"/>
       <c r="D215" s="7"/>
       <c r="E215" s="4"/>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" s="7"/>
+    <row r="216" spans="1:5">
+      <c r="A216" s="4"/>
       <c r="B216" s="7"/>
       <c r="C216" s="7"/>
       <c r="D216" s="7"/>
       <c r="E216" s="4"/>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A217" s="7"/>
+    <row r="217" spans="1:5">
+      <c r="A217" s="4"/>
       <c r="B217" s="7"/>
       <c r="C217" s="7"/>
       <c r="D217" s="7"/>
       <c r="E217" s="4"/>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A218" s="7"/>
+    <row r="218" spans="1:5">
+      <c r="A218" s="4"/>
       <c r="B218" s="7"/>
       <c r="C218" s="7"/>
       <c r="D218" s="7"/>
       <c r="E218" s="4"/>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A219" s="7"/>
+    <row r="219" spans="1:5">
+      <c r="A219" s="4"/>
       <c r="B219" s="7"/>
       <c r="C219" s="7"/>
       <c r="D219" s="7"/>
       <c r="E219" s="4"/>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A220" s="7"/>
+    <row r="220" spans="1:5">
+      <c r="A220" s="4"/>
       <c r="B220" s="7"/>
       <c r="C220" s="7"/>
       <c r="D220" s="7"/>
       <c r="E220" s="4"/>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A221" s="7"/>
+    <row r="221" spans="1:5">
+      <c r="A221" s="4"/>
       <c r="B221" s="7"/>
       <c r="C221" s="7"/>
       <c r="D221" s="7"/>
       <c r="E221" s="4"/>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" s="7"/>
+    <row r="222" spans="1:5">
+      <c r="A222" s="4"/>
       <c r="B222" s="7"/>
       <c r="C222" s="7"/>
       <c r="D222" s="7"/>
       <c r="E222" s="4"/>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A223" s="7"/>
+    <row r="223" spans="1:5">
+      <c r="A223" s="4"/>
       <c r="B223" s="7"/>
       <c r="C223" s="7"/>
       <c r="D223" s="7"/>
       <c r="E223" s="4"/>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A224" s="7"/>
+    <row r="224" spans="1:5">
+      <c r="A224" s="4"/>
       <c r="B224" s="7"/>
       <c r="C224" s="7"/>
       <c r="D224" s="7"/>
       <c r="E224" s="4"/>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A225" s="7"/>
+    <row r="225" spans="1:5">
+      <c r="A225" s="4"/>
       <c r="B225" s="7"/>
       <c r="C225" s="7"/>
       <c r="D225" s="7"/>
       <c r="E225" s="4"/>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A226" s="7"/>
+    <row r="226" spans="1:5">
+      <c r="A226" s="4"/>
       <c r="B226" s="7"/>
       <c r="C226" s="7"/>
       <c r="D226" s="7"/>
       <c r="E226" s="4"/>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A227" s="7"/>
+    <row r="227" spans="1:5">
+      <c r="A227" s="4"/>
       <c r="B227" s="7"/>
       <c r="C227" s="7"/>
       <c r="D227" s="7"/>
       <c r="E227" s="4"/>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A228" s="7"/>
+    <row r="228" spans="1:5">
+      <c r="A228" s="4"/>
       <c r="B228" s="7"/>
       <c r="C228" s="7"/>
       <c r="D228" s="7"/>
       <c r="E228" s="4"/>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A229" s="7"/>
+    <row r="229" spans="1:5">
+      <c r="A229" s="4"/>
       <c r="B229" s="7"/>
       <c r="C229" s="7"/>
       <c r="D229" s="7"/>
       <c r="E229" s="4"/>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A230" s="7"/>
+    <row r="230" spans="1:5">
+      <c r="A230" s="4"/>
       <c r="B230" s="7"/>
       <c r="C230" s="7"/>
       <c r="D230" s="7"/>
       <c r="E230" s="4"/>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A231" s="7"/>
+    <row r="231" spans="1:5">
+      <c r="A231" s="4"/>
       <c r="B231" s="7"/>
       <c r="C231" s="7"/>
       <c r="D231" s="7"/>
       <c r="E231" s="4"/>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A232" s="7"/>
+    <row r="232" spans="1:5">
+      <c r="A232" s="4"/>
       <c r="B232" s="7"/>
       <c r="C232" s="7"/>
       <c r="D232" s="7"/>
       <c r="E232" s="4"/>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A233" s="7"/>
+    <row r="233" spans="1:5">
+      <c r="A233" s="4"/>
       <c r="B233" s="7"/>
       <c r="C233" s="7"/>
       <c r="D233" s="7"/>
       <c r="E233" s="4"/>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A234" s="7"/>
+    <row r="234" spans="1:5">
+      <c r="A234" s="4"/>
       <c r="B234" s="7"/>
       <c r="C234" s="7"/>
       <c r="D234" s="7"/>
       <c r="E234" s="4"/>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A235" s="7"/>
+    <row r="235" spans="1:5">
+      <c r="A235" s="4"/>
       <c r="B235" s="7"/>
       <c r="C235" s="7"/>
       <c r="D235" s="7"/>
       <c r="E235" s="4"/>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A236" s="7"/>
+    <row r="236" spans="1:5">
+      <c r="A236" s="4"/>
       <c r="B236" s="7"/>
       <c r="C236" s="7"/>
       <c r="D236" s="7"/>
       <c r="E236" s="4"/>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A237" s="7"/>
+    <row r="237" spans="1:5">
+      <c r="A237" s="4"/>
       <c r="B237" s="7"/>
       <c r="C237" s="7"/>
       <c r="D237" s="7"/>
       <c r="E237" s="4"/>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A238" s="7"/>
+    <row r="238" spans="1:5">
+      <c r="A238" s="4"/>
       <c r="B238" s="7"/>
       <c r="C238" s="7"/>
       <c r="D238" s="7"/>
       <c r="E238" s="4"/>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A239" s="7"/>
+    <row r="239" spans="1:5">
+      <c r="A239" s="4"/>
       <c r="B239" s="7"/>
       <c r="C239" s="7"/>
       <c r="D239" s="7"/>
       <c r="E239" s="4"/>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A240" s="7"/>
+    <row r="240" spans="1:5">
+      <c r="A240" s="4"/>
       <c r="B240" s="7"/>
       <c r="C240" s="7"/>
       <c r="D240" s="7"/>
       <c r="E240" s="4"/>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A241" s="7"/>
+    <row r="241" spans="1:5">
+      <c r="A241" s="4"/>
       <c r="B241" s="7"/>
       <c r="C241" s="7"/>
       <c r="D241" s="7"/>
       <c r="E241" s="4"/>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A242" s="7"/>
+    <row r="242" spans="1:5">
+      <c r="A242" s="4"/>
       <c r="B242" s="7"/>
       <c r="C242" s="7"/>
       <c r="D242" s="7"/>
       <c r="E242" s="4"/>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A243" s="7"/>
+    <row r="243" spans="1:5">
+      <c r="A243" s="4"/>
       <c r="B243" s="7"/>
       <c r="C243" s="7"/>
       <c r="D243" s="7"/>
       <c r="E243" s="4"/>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A244" s="7"/>
+    <row r="244" spans="1:5">
+      <c r="A244" s="4"/>
       <c r="B244" s="7"/>
       <c r="C244" s="7"/>
       <c r="D244" s="7"/>
       <c r="E244" s="4"/>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A245" s="7"/>
+    <row r="245" spans="1:5">
+      <c r="A245" s="4"/>
       <c r="B245" s="7"/>
       <c r="C245" s="7"/>
       <c r="D245" s="7"/>
       <c r="E245" s="4"/>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A246" s="7"/>
+    <row r="246" spans="1:5">
+      <c r="A246" s="4"/>
       <c r="B246" s="7"/>
       <c r="C246" s="7"/>
       <c r="D246" s="7"/>
       <c r="E246" s="4"/>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A247" s="7"/>
+    <row r="247" spans="1:5">
+      <c r="A247" s="4"/>
       <c r="B247" s="7"/>
       <c r="C247" s="7"/>
       <c r="D247" s="7"/>
       <c r="E247" s="4"/>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A248" s="7"/>
+    <row r="248" spans="1:5">
+      <c r="A248" s="4"/>
       <c r="B248" s="7"/>
       <c r="C248" s="7"/>
       <c r="D248" s="7"/>
       <c r="E248" s="4"/>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A249" s="7"/>
+    <row r="249" spans="1:5">
+      <c r="A249" s="4"/>
       <c r="B249" s="7"/>
       <c r="C249" s="7"/>
       <c r="D249" s="7"/>
       <c r="E249" s="4"/>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A250" s="7"/>
+    <row r="250" spans="1:5">
+      <c r="A250" s="4"/>
       <c r="B250" s="7"/>
       <c r="C250" s="7"/>
       <c r="D250" s="7"/>
       <c r="E250" s="4"/>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A251" s="7"/>
+    <row r="251" spans="1:5">
+      <c r="A251" s="4"/>
       <c r="B251" s="7"/>
       <c r="C251" s="7"/>
       <c r="D251" s="7"/>
       <c r="E251" s="4"/>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A252" s="7"/>
+    <row r="252" spans="1:5">
+      <c r="A252" s="4"/>
       <c r="B252" s="7"/>
       <c r="C252" s="7"/>
       <c r="D252" s="7"/>
       <c r="E252" s="4"/>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A253" s="7"/>
+    <row r="253" spans="1:5">
+      <c r="A253" s="4"/>
       <c r="B253" s="7"/>
       <c r="C253" s="7"/>
       <c r="D253" s="7"/>
       <c r="E253" s="4"/>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A254" s="7"/>
+    <row r="254" spans="1:5">
+      <c r="A254" s="4"/>
       <c r="B254" s="7"/>
       <c r="C254" s="7"/>
       <c r="D254" s="7"/>
       <c r="E254" s="4"/>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A255" s="7"/>
+    <row r="255" spans="1:5">
+      <c r="A255" s="4"/>
       <c r="B255" s="7"/>
       <c r="C255" s="7"/>
       <c r="D255" s="7"/>
       <c r="E255" s="4"/>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A256" s="7"/>
+    <row r="256" spans="1:5">
+      <c r="A256" s="4"/>
       <c r="B256" s="7"/>
       <c r="C256" s="7"/>
       <c r="D256" s="7"/>
       <c r="E256" s="4"/>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A257" s="7"/>
+    <row r="257" spans="1:5">
+      <c r="A257" s="4"/>
       <c r="B257" s="7"/>
       <c r="C257" s="7"/>
       <c r="D257" s="7"/>
       <c r="E257" s="4"/>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A258" s="7"/>
+    <row r="258" spans="1:5">
+      <c r="A258" s="4"/>
       <c r="B258" s="7"/>
       <c r="C258" s="7"/>
       <c r="D258" s="7"/>
       <c r="E258" s="4"/>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A259" s="7"/>
+    <row r="259" spans="1:5">
+      <c r="A259" s="4"/>
       <c r="B259" s="7"/>
       <c r="C259" s="7"/>
       <c r="D259" s="7"/>
       <c r="E259" s="4"/>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A260" s="7"/>
+    <row r="260" spans="1:5">
+      <c r="A260" s="4"/>
       <c r="B260" s="7"/>
       <c r="C260" s="7"/>
       <c r="D260" s="7"/>
       <c r="E260" s="4"/>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A261" s="7"/>
+    <row r="261" spans="1:5">
+      <c r="A261" s="4"/>
       <c r="B261" s="7"/>
       <c r="C261" s="7"/>
       <c r="D261" s="7"/>
       <c r="E261" s="4"/>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A262" s="7"/>
+    <row r="262" spans="1:5">
+      <c r="A262" s="4"/>
       <c r="B262" s="7"/>
       <c r="C262" s="7"/>
       <c r="D262" s="7"/>
       <c r="E262" s="4"/>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A263" s="7"/>
+    <row r="263" spans="1:5">
+      <c r="A263" s="4"/>
       <c r="B263" s="7"/>
       <c r="C263" s="7"/>
       <c r="D263" s="7"/>
       <c r="E263" s="4"/>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A264" s="7"/>
+    <row r="264" spans="1:5">
+      <c r="A264" s="4"/>
       <c r="B264" s="7"/>
       <c r="C264" s="7"/>
       <c r="D264" s="7"/>
       <c r="E264" s="4"/>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A265" s="7"/>
+    <row r="265" spans="1:5">
+      <c r="A265" s="4"/>
       <c r="B265" s="7"/>
       <c r="C265" s="7"/>
       <c r="D265" s="7"/>
       <c r="E265" s="4"/>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A266" s="7"/>
+    <row r="266" spans="1:5">
+      <c r="A266" s="4"/>
       <c r="B266" s="7"/>
       <c r="C266" s="7"/>
       <c r="D266" s="7"/>
       <c r="E266" s="4"/>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A267" s="7"/>
+    <row r="267" spans="1:5">
+      <c r="A267" s="4"/>
       <c r="B267" s="7"/>
       <c r="C267" s="7"/>
       <c r="D267" s="7"/>
       <c r="E267" s="4"/>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A268" s="7"/>
+    <row r="268" spans="1:5">
+      <c r="A268" s="4"/>
       <c r="B268" s="7"/>
       <c r="C268" s="7"/>
       <c r="D268" s="7"/>
       <c r="E268" s="4"/>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A269" s="7"/>
+    <row r="269" spans="1:5">
+      <c r="A269" s="4"/>
       <c r="B269" s="7"/>
       <c r="C269" s="7"/>
       <c r="D269" s="7"/>
       <c r="E269" s="4"/>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A270" s="7"/>
+    <row r="270" spans="1:5">
+      <c r="A270" s="4"/>
       <c r="B270" s="7"/>
       <c r="C270" s="7"/>
       <c r="D270" s="7"/>
       <c r="E270" s="4"/>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A271" s="7"/>
+    <row r="271" spans="1:5">
+      <c r="A271" s="4"/>
       <c r="B271" s="7"/>
       <c r="C271" s="7"/>
       <c r="D271" s="7"/>
       <c r="E271" s="4"/>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A272" s="7"/>
+    <row r="272" spans="1:5">
+      <c r="A272" s="4"/>
       <c r="B272" s="7"/>
       <c r="C272" s="7"/>
       <c r="D272" s="7"/>
       <c r="E272" s="4"/>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A273" s="7"/>
+    <row r="273" spans="1:5">
+      <c r="A273" s="4"/>
       <c r="B273" s="7"/>
       <c r="C273" s="7"/>
       <c r="D273" s="7"/>
       <c r="E273" s="4"/>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A274" s="7"/>
+    <row r="274" spans="1:5">
+      <c r="A274" s="4"/>
       <c r="B274" s="7"/>
       <c r="C274" s="7"/>
       <c r="D274" s="7"/>
       <c r="E274" s="4"/>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A275" s="7"/>
+    <row r="275" spans="1:5">
+      <c r="A275" s="4"/>
       <c r="B275" s="7"/>
       <c r="C275" s="7"/>
       <c r="D275" s="7"/>
       <c r="E275" s="4"/>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A276" s="7"/>
+    <row r="276" spans="1:5">
+      <c r="A276" s="4"/>
       <c r="B276" s="7"/>
       <c r="C276" s="7"/>
       <c r="D276" s="7"/>
       <c r="E276" s="4"/>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A277" s="7"/>
+    <row r="277" spans="1:5">
+      <c r="A277" s="4"/>
       <c r="B277" s="7"/>
       <c r="C277" s="7"/>
       <c r="D277" s="7"/>
       <c r="E277" s="4"/>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A278" s="7"/>
+    <row r="278" spans="1:5">
+      <c r="A278" s="4"/>
       <c r="B278" s="7"/>
       <c r="C278" s="7"/>
       <c r="D278" s="7"/>
       <c r="E278" s="4"/>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A279" s="7"/>
+    <row r="279" spans="1:5">
+      <c r="A279" s="4"/>
       <c r="B279" s="7"/>
       <c r="C279" s="7"/>
       <c r="D279" s="7"/>
       <c r="E279" s="4"/>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A280" s="7"/>
+    <row r="280" spans="1:5">
+      <c r="A280" s="4"/>
       <c r="B280" s="7"/>
       <c r="C280" s="7"/>
       <c r="D280" s="7"/>
       <c r="E280" s="4"/>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A281" s="7"/>
+    <row r="281" spans="1:5">
+      <c r="A281" s="4"/>
       <c r="B281" s="7"/>
       <c r="C281" s="7"/>
       <c r="D281" s="7"/>
       <c r="E281" s="4"/>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A282" s="7"/>
+    <row r="282" spans="1:5">
+      <c r="A282" s="4"/>
       <c r="B282" s="7"/>
       <c r="C282" s="7"/>
       <c r="D282" s="7"/>
       <c r="E282" s="4"/>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A283" s="7"/>
+    <row r="283" spans="1:5">
+      <c r="A283" s="4"/>
       <c r="B283" s="7"/>
       <c r="C283" s="7"/>
       <c r="D283" s="7"/>
       <c r="E283" s="4"/>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A284" s="7"/>
+    <row r="284" spans="1:5">
+      <c r="A284" s="4"/>
       <c r="B284" s="7"/>
       <c r="C284" s="7"/>
       <c r="D284" s="7"/>
       <c r="E284" s="4"/>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A285" s="7"/>
+    <row r="285" spans="1:5">
+      <c r="A285" s="4"/>
       <c r="B285" s="7"/>
       <c r="C285" s="7"/>
       <c r="D285" s="7"/>
       <c r="E285" s="4"/>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A286" s="7"/>
+    <row r="286" spans="1:5">
+      <c r="A286" s="4"/>
       <c r="B286" s="7"/>
       <c r="C286" s="7"/>
       <c r="D286" s="7"/>
       <c r="E286" s="4"/>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A287" s="7"/>
+    <row r="287" spans="1:5">
+      <c r="A287" s="4"/>
       <c r="B287" s="7"/>
       <c r="C287" s="7"/>
       <c r="D287" s="7"/>
       <c r="E287" s="4"/>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A288" s="7"/>
+    <row r="288" spans="1:5">
+      <c r="A288" s="4"/>
       <c r="B288" s="7"/>
       <c r="C288" s="7"/>
       <c r="D288" s="7"/>
       <c r="E288" s="4"/>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A289" s="7"/>
+    <row r="289" spans="1:5">
+      <c r="A289" s="4"/>
       <c r="B289" s="7"/>
       <c r="C289" s="7"/>
       <c r="D289" s="7"/>
       <c r="E289" s="4"/>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A290" s="7"/>
+    <row r="290" spans="1:5">
+      <c r="A290" s="4"/>
       <c r="B290" s="7"/>
       <c r="C290" s="7"/>
       <c r="D290" s="7"/>
       <c r="E290" s="4"/>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A291" s="7"/>
+    <row r="291" spans="1:5">
+      <c r="A291" s="4"/>
       <c r="B291" s="7"/>
       <c r="C291" s="7"/>
       <c r="D291" s="7"/>
       <c r="E291" s="4"/>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A292" s="7"/>
+    <row r="292" spans="1:5">
+      <c r="A292" s="4"/>
       <c r="B292" s="7"/>
       <c r="C292" s="7"/>
       <c r="D292" s="7"/>
       <c r="E292" s="4"/>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A293" s="7"/>
+    <row r="293" spans="1:5">
+      <c r="A293" s="4"/>
       <c r="B293" s="7"/>
       <c r="C293" s="7"/>
       <c r="D293" s="7"/>
       <c r="E293" s="4"/>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A294" s="7"/>
+    <row r="294" spans="1:5">
+      <c r="A294" s="4"/>
       <c r="B294" s="7"/>
       <c r="C294" s="7"/>
       <c r="D294" s="7"/>
       <c r="E294" s="4"/>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A295" s="7"/>
+    <row r="295" spans="1:5">
+      <c r="A295" s="4"/>
       <c r="B295" s="7"/>
       <c r="C295" s="7"/>
       <c r="D295" s="7"/>
       <c r="E295" s="4"/>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A296" s="7"/>
+    <row r="296" spans="1:5">
+      <c r="A296" s="4"/>
       <c r="B296" s="7"/>
       <c r="C296" s="7"/>
       <c r="D296" s="7"/>
       <c r="E296" s="4"/>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A297" s="7"/>
+    <row r="297" spans="1:5">
+      <c r="A297" s="4"/>
       <c r="B297" s="7"/>
       <c r="C297" s="7"/>
       <c r="D297" s="7"/>
       <c r="E297" s="4"/>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A298" s="7"/>
+    <row r="298" spans="1:5">
+      <c r="A298" s="4"/>
       <c r="B298" s="7"/>
       <c r="C298" s="7"/>
       <c r="D298" s="7"/>
       <c r="E298" s="4"/>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="7"/>
+    <row r="299" spans="1:5">
+      <c r="A299" s="4"/>
       <c r="B299" s="7"/>
       <c r="C299" s="7"/>
       <c r="D299" s="7"/>
       <c r="E299" s="4"/>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A300" s="7"/>
+    <row r="300" spans="1:5">
+      <c r="A300" s="4"/>
       <c r="B300" s="7"/>
       <c r="C300" s="7"/>
       <c r="D300" s="7"/>
       <c r="E300" s="4"/>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A301" s="7"/>
+    <row r="301" spans="1:5">
+      <c r="A301" s="4"/>
       <c r="B301" s="7"/>
       <c r="C301" s="7"/>
       <c r="D301" s="7"/>
       <c r="E301" s="4"/>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A302" s="7"/>
+    <row r="302" spans="1:5">
+      <c r="A302" s="4"/>
       <c r="B302" s="7"/>
       <c r="C302" s="7"/>
       <c r="D302" s="7"/>
       <c r="E302" s="4"/>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A303" s="7"/>
+    <row r="303" spans="1:5">
+      <c r="A303" s="4"/>
       <c r="B303" s="7"/>
       <c r="C303" s="7"/>
       <c r="D303" s="7"/>
       <c r="E303" s="4"/>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A304" s="7"/>
+    <row r="304" spans="1:5">
+      <c r="A304" s="4"/>
       <c r="B304" s="7"/>
       <c r="C304" s="7"/>
       <c r="D304" s="7"/>
       <c r="E304" s="4"/>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A305" s="7"/>
+    <row r="305" spans="1:5">
+      <c r="A305" s="4"/>
       <c r="B305" s="7"/>
       <c r="C305" s="7"/>
       <c r="D305" s="7"/>
       <c r="E305" s="4"/>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A306" s="7"/>
+    <row r="306" spans="1:5">
+      <c r="A306" s="4"/>
       <c r="B306" s="7"/>
       <c r="C306" s="7"/>
       <c r="D306" s="7"/>
       <c r="E306" s="4"/>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A307" s="7"/>
+    <row r="307" spans="1:5">
+      <c r="A307" s="4"/>
       <c r="B307" s="7"/>
       <c r="C307" s="7"/>
       <c r="D307" s="7"/>
       <c r="E307" s="4"/>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A308" s="7"/>
+    <row r="308" spans="1:5">
+      <c r="A308" s="4"/>
       <c r="B308" s="7"/>
       <c r="C308" s="7"/>
       <c r="D308" s="7"/>
       <c r="E308" s="4"/>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A309" s="7"/>
+    <row r="309" spans="1:5">
+      <c r="A309" s="4"/>
       <c r="B309" s="7"/>
       <c r="C309" s="7"/>
       <c r="D309" s="7"/>
       <c r="E309" s="4"/>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A310" s="7"/>
+    <row r="310" spans="1:5">
+      <c r="A310" s="4"/>
       <c r="B310" s="7"/>
       <c r="C310" s="7"/>
       <c r="D310" s="7"/>
       <c r="E310" s="4"/>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A311" s="7"/>
+    <row r="311" spans="1:5">
+      <c r="A311" s="4"/>
       <c r="B311" s="7"/>
       <c r="C311" s="7"/>
       <c r="D311" s="7"/>
       <c r="E311" s="4"/>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A312" s="7"/>
+    <row r="312" spans="1:5">
+      <c r="A312" s="4"/>
       <c r="B312" s="7"/>
       <c r="C312" s="7"/>
       <c r="D312" s="7"/>
       <c r="E312" s="4"/>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A313" s="7"/>
+    <row r="313" spans="1:5">
+      <c r="A313" s="4"/>
       <c r="B313" s="7"/>
       <c r="C313" s="7"/>
       <c r="D313" s="7"/>
       <c r="E313" s="4"/>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A314" s="7"/>
+    <row r="314" spans="1:5">
+      <c r="A314" s="4"/>
       <c r="B314" s="7"/>
       <c r="C314" s="7"/>
       <c r="D314" s="7"/>
       <c r="E314" s="4"/>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A315" s="7"/>
+    <row r="315" spans="1:5">
+      <c r="A315" s="4"/>
       <c r="B315" s="7"/>
       <c r="C315" s="7"/>
       <c r="D315" s="7"/>
       <c r="E315" s="4"/>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A316" s="7"/>
+    <row r="316" spans="1:5">
+      <c r="A316" s="4"/>
       <c r="B316" s="7"/>
       <c r="C316" s="7"/>
       <c r="D316" s="7"/>
       <c r="E316" s="4"/>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A317" s="7"/>
+    <row r="317" spans="1:5">
+      <c r="A317" s="4"/>
       <c r="B317" s="7"/>
       <c r="C317" s="7"/>
       <c r="D317" s="7"/>
       <c r="E317" s="4"/>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A318" s="7"/>
+    <row r="318" spans="1:5">
+      <c r="A318" s="4"/>
       <c r="B318" s="7"/>
       <c r="C318" s="7"/>
       <c r="D318" s="7"/>
       <c r="E318" s="4"/>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A319" s="7"/>
+    <row r="319" spans="1:5">
+      <c r="A319" s="4"/>
       <c r="B319" s="7"/>
       <c r="C319" s="7"/>
       <c r="D319" s="7"/>
       <c r="E319" s="4"/>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A320" s="7"/>
+    <row r="320" spans="1:5">
+      <c r="A320" s="4"/>
       <c r="B320" s="7"/>
       <c r="C320" s="7"/>
       <c r="D320" s="7"/>
       <c r="E320" s="4"/>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A321" s="7"/>
+    <row r="321" spans="1:5">
+      <c r="A321" s="4"/>
       <c r="B321" s="7"/>
       <c r="C321" s="7"/>
       <c r="D321" s="7"/>
       <c r="E321" s="4"/>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A322" s="7"/>
+    <row r="322" spans="1:5">
+      <c r="A322" s="4"/>
       <c r="B322" s="7"/>
       <c r="C322" s="7"/>
       <c r="D322" s="7"/>
       <c r="E322" s="4"/>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A323" s="7"/>
+    <row r="323" spans="1:5">
+      <c r="A323" s="4"/>
       <c r="B323" s="7"/>
       <c r="C323" s="7"/>
       <c r="D323" s="7"/>
       <c r="E323" s="4"/>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A324" s="7"/>
+    <row r="324" spans="1:5">
+      <c r="A324" s="4"/>
       <c r="B324" s="7"/>
       <c r="C324" s="7"/>
       <c r="D324" s="7"/>
       <c r="E324" s="4"/>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A325" s="7"/>
+    <row r="325" spans="1:5">
+      <c r="A325" s="4"/>
       <c r="B325" s="7"/>
       <c r="C325" s="7"/>
       <c r="D325" s="7"/>
       <c r="E325" s="4"/>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A326" s="7"/>
+    <row r="326" spans="1:5">
+      <c r="A326" s="4"/>
       <c r="B326" s="7"/>
       <c r="C326" s="7"/>
       <c r="D326" s="7"/>
       <c r="E326" s="4"/>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A327" s="7"/>
+    <row r="327" spans="1:5">
+      <c r="A327" s="4"/>
       <c r="B327" s="7"/>
       <c r="C327" s="7"/>
       <c r="D327" s="7"/>
       <c r="E327" s="4"/>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A328" s="7"/>
+    <row r="328" spans="1:5">
+      <c r="A328" s="4"/>
       <c r="B328" s="7"/>
       <c r="C328" s="7"/>
       <c r="D328" s="7"/>
       <c r="E328" s="4"/>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A329" s="7"/>
+    <row r="329" spans="1:5">
+      <c r="A329" s="4"/>
       <c r="B329" s="7"/>
       <c r="C329" s="7"/>
       <c r="D329" s="7"/>
       <c r="E329" s="4"/>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A330" s="7"/>
+    <row r="330" spans="1:5">
+      <c r="A330" s="4"/>
       <c r="B330" s="7"/>
       <c r="C330" s="7"/>
       <c r="D330" s="7"/>
       <c r="E330" s="4"/>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A331" s="7"/>
+    <row r="331" spans="1:5">
+      <c r="A331" s="4"/>
       <c r="B331" s="7"/>
       <c r="C331" s="7"/>
       <c r="D331" s="7"/>
       <c r="E331" s="4"/>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A332" s="7"/>
+    <row r="332" spans="1:5">
+      <c r="A332" s="4"/>
       <c r="B332" s="7"/>
       <c r="C332" s="7"/>
       <c r="D332" s="7"/>
       <c r="E332" s="4"/>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A333" s="7"/>
+    <row r="333" spans="1:5">
+      <c r="A333" s="4"/>
       <c r="B333" s="7"/>
       <c r="C333" s="7"/>
       <c r="D333" s="7"/>
       <c r="E333" s="4"/>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A334" s="7"/>
+    <row r="334" spans="1:5">
+      <c r="A334" s="4"/>
       <c r="B334" s="7"/>
       <c r="C334" s="7"/>
       <c r="D334" s="7"/>
       <c r="E334" s="4"/>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A335" s="7"/>
+    <row r="335" spans="1:5">
+      <c r="A335" s="4"/>
       <c r="B335" s="7"/>
       <c r="C335" s="7"/>
       <c r="D335" s="7"/>
       <c r="E335" s="4"/>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A336" s="7"/>
+    <row r="336" spans="1:5">
+      <c r="A336" s="4"/>
       <c r="B336" s="7"/>
       <c r="C336" s="7"/>
       <c r="D336" s="7"/>
       <c r="E336" s="4"/>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A337" s="7"/>
+    <row r="337" spans="1:5">
+      <c r="A337" s="4"/>
       <c r="B337" s="7"/>
       <c r="C337" s="7"/>
       <c r="D337" s="7"/>
       <c r="E337" s="4"/>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A338" s="7"/>
+    <row r="338" spans="1:5">
+      <c r="A338" s="4"/>
       <c r="B338" s="7"/>
       <c r="C338" s="7"/>
       <c r="D338" s="7"/>
       <c r="E338" s="4"/>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A339" s="7"/>
+    <row r="339" spans="1:5">
+      <c r="A339" s="4"/>
       <c r="B339" s="7"/>
       <c r="C339" s="7"/>
       <c r="D339" s="7"/>
       <c r="E339" s="4"/>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A340" s="7"/>
+    <row r="340" spans="1:5">
+      <c r="A340" s="4"/>
       <c r="B340" s="7"/>
       <c r="C340" s="7"/>
       <c r="D340" s="7"/>
       <c r="E340" s="4"/>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A341" s="7"/>
+    <row r="341" spans="1:5">
+      <c r="A341" s="4"/>
       <c r="B341" s="7"/>
       <c r="C341" s="7"/>
       <c r="D341" s="7"/>
       <c r="E341" s="4"/>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A342" s="7"/>
+    <row r="342" spans="1:5">
+      <c r="A342" s="4"/>
       <c r="B342" s="7"/>
       <c r="C342" s="7"/>
       <c r="D342" s="7"/>
       <c r="E342" s="4"/>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A343" s="7"/>
+    <row r="343" spans="1:5">
+      <c r="A343" s="4"/>
       <c r="B343" s="7"/>
       <c r="C343" s="7"/>
       <c r="D343" s="7"/>
       <c r="E343" s="4"/>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A344" s="7"/>
+    <row r="344" spans="1:5">
+      <c r="A344" s="4"/>
       <c r="B344" s="7"/>
       <c r="C344" s="7"/>
       <c r="D344" s="7"/>
       <c r="E344" s="4"/>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A345" s="7"/>
+    <row r="345" spans="1:5">
+      <c r="A345" s="4"/>
       <c r="B345" s="7"/>
       <c r="C345" s="7"/>
       <c r="D345" s="7"/>
       <c r="E345" s="4"/>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A346" s="7"/>
+    <row r="346" spans="1:5">
+      <c r="A346" s="4"/>
       <c r="B346" s="7"/>
       <c r="C346" s="7"/>
       <c r="D346" s="7"/>
       <c r="E346" s="4"/>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A347" s="7"/>
+    <row r="347" spans="1:5">
+      <c r="A347" s="4"/>
       <c r="B347" s="7"/>
       <c r="C347" s="7"/>
       <c r="D347" s="7"/>
       <c r="E347" s="4"/>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A348" s="7"/>
+    <row r="348" spans="1:5">
+      <c r="A348" s="4"/>
       <c r="B348" s="7"/>
       <c r="C348" s="7"/>
       <c r="D348" s="7"/>
       <c r="E348" s="4"/>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A349" s="7"/>
+    <row r="349" spans="1:5">
+      <c r="A349" s="4"/>
       <c r="B349" s="7"/>
       <c r="C349" s="7"/>
       <c r="D349" s="7"/>
       <c r="E349" s="4"/>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A350" s="7"/>
+    <row r="350" spans="1:5">
+      <c r="A350" s="4"/>
       <c r="B350" s="7"/>
       <c r="C350" s="7"/>
       <c r="D350" s="7"/>
       <c r="E350" s="4"/>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A351" s="7"/>
+    <row r="351" spans="1:5">
+      <c r="A351" s="4"/>
       <c r="B351" s="7"/>
       <c r="C351" s="7"/>
       <c r="D351" s="7"/>
       <c r="E351" s="4"/>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A352" s="7"/>
+    <row r="352" spans="1:5">
+      <c r="A352" s="4"/>
       <c r="B352" s="7"/>
       <c r="C352" s="7"/>
       <c r="D352" s="7"/>
       <c r="E352" s="4"/>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A353" s="7"/>
+    <row r="353" spans="1:5">
+      <c r="A353" s="4"/>
       <c r="B353" s="7"/>
       <c r="C353" s="7"/>
       <c r="D353" s="7"/>
       <c r="E353" s="4"/>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A354" s="7"/>
+    <row r="354" spans="1:5">
+      <c r="A354" s="4"/>
       <c r="B354" s="7"/>
       <c r="C354" s="7"/>
       <c r="D354" s="7"/>
       <c r="E354" s="4"/>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A355" s="7"/>
+    <row r="355" spans="1:5">
+      <c r="A355" s="4"/>
       <c r="B355" s="7"/>
       <c r="C355" s="7"/>
       <c r="D355" s="7"/>
       <c r="E355" s="4"/>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A356" s="7"/>
+    <row r="356" spans="1:5">
+      <c r="A356" s="4"/>
       <c r="B356" s="7"/>
       <c r="C356" s="7"/>
       <c r="D356" s="7"/>
       <c r="E356" s="4"/>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A357" s="7"/>
+    <row r="357" spans="1:5">
+      <c r="A357" s="4"/>
       <c r="B357" s="7"/>
       <c r="C357" s="7"/>
       <c r="D357" s="7"/>
       <c r="E357" s="4"/>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A358" s="7"/>
+    <row r="358" spans="1:5">
+      <c r="A358" s="4"/>
       <c r="B358" s="7"/>
       <c r="C358" s="7"/>
       <c r="D358" s="7"/>
       <c r="E358" s="4"/>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A359" s="7"/>
+    <row r="359" spans="1:5">
+      <c r="A359" s="4"/>
       <c r="B359" s="7"/>
       <c r="C359" s="7"/>
       <c r="D359" s="7"/>
       <c r="E359" s="4"/>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A360" s="7"/>
+    <row r="360" spans="1:5">
+      <c r="A360" s="4"/>
       <c r="B360" s="7"/>
       <c r="C360" s="7"/>
       <c r="D360" s="7"/>
       <c r="E360" s="4"/>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A361" s="7"/>
+    <row r="361" spans="1:5">
+      <c r="A361" s="4"/>
       <c r="B361" s="7"/>
       <c r="C361" s="7"/>
       <c r="D361" s="7"/>
       <c r="E361" s="4"/>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A362" s="7"/>
+    <row r="362" spans="1:5">
+      <c r="A362" s="4"/>
       <c r="B362" s="7"/>
       <c r="C362" s="7"/>
       <c r="D362" s="7"/>
       <c r="E362" s="4"/>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A363" s="7"/>
+    <row r="363" spans="1:5">
+      <c r="A363" s="4"/>
       <c r="B363" s="7"/>
       <c r="C363" s="7"/>
       <c r="D363" s="7"/>
       <c r="E363" s="4"/>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A364" s="7"/>
+    <row r="364" spans="1:5">
+      <c r="A364" s="4"/>
       <c r="B364" s="7"/>
       <c r="C364" s="7"/>
       <c r="D364" s="7"/>
       <c r="E364" s="4"/>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A365" s="7"/>
+    <row r="365" spans="1:5">
+      <c r="A365" s="4"/>
       <c r="B365" s="7"/>
       <c r="C365" s="7"/>
       <c r="D365" s="7"/>
       <c r="E365" s="4"/>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A366" s="7"/>
+    <row r="366" spans="1:5">
+      <c r="A366" s="4"/>
       <c r="B366" s="7"/>
       <c r="C366" s="7"/>
       <c r="D366" s="7"/>
       <c r="E366" s="4"/>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A367" s="7"/>
+    <row r="367" spans="1:5">
+      <c r="A367" s="4"/>
       <c r="B367" s="7"/>
       <c r="C367" s="7"/>
       <c r="D367" s="7"/>
       <c r="E367" s="4"/>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A368" s="7"/>
+    <row r="368" spans="1:5">
+      <c r="A368" s="4"/>
       <c r="B368" s="7"/>
       <c r="C368" s="7"/>
       <c r="D368" s="7"/>
       <c r="E368" s="4"/>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A369" s="7"/>
+    <row r="369" spans="1:5">
+      <c r="A369" s="4"/>
       <c r="B369" s="7"/>
       <c r="C369" s="7"/>
       <c r="D369" s="7"/>
       <c r="E369" s="4"/>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A370" s="7"/>
+    <row r="370" spans="1:5">
+      <c r="A370" s="4"/>
       <c r="B370" s="7"/>
       <c r="C370" s="7"/>
       <c r="D370" s="7"/>
       <c r="E370" s="4"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A371" s="7"/>
+    <row r="371" spans="1:5">
+      <c r="A371" s="4"/>
       <c r="B371" s="7"/>
       <c r="C371" s="7"/>
       <c r="D371" s="7"/>
       <c r="E371" s="4"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A372" s="7"/>
+    <row r="372" spans="1:5">
+      <c r="A372" s="4"/>
       <c r="B372" s="7"/>
       <c r="C372" s="7"/>
       <c r="D372" s="7"/>
       <c r="E372" s="4"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A373" s="7"/>
+    <row r="373" spans="1:5">
+      <c r="A373" s="4"/>
       <c r="B373" s="7"/>
       <c r="C373" s="7"/>
       <c r="D373" s="7"/>
       <c r="E373" s="4"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A374" s="7"/>
+    <row r="374" spans="1:5">
+      <c r="A374" s="4"/>
       <c r="B374" s="7"/>
       <c r="C374" s="7"/>
       <c r="D374" s="7"/>
       <c r="E374" s="4"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A375" s="7"/>
+    <row r="375" spans="1:5">
+      <c r="A375" s="4"/>
       <c r="B375" s="7"/>
       <c r="C375" s="7"/>
       <c r="D375" s="7"/>
       <c r="E375" s="4"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A376" s="7"/>
+    <row r="376" spans="1:5">
+      <c r="A376" s="4"/>
       <c r="B376" s="7"/>
       <c r="C376" s="7"/>
       <c r="D376" s="7"/>
       <c r="E376" s="4"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A377" s="7"/>
+    <row r="377" spans="1:5">
+      <c r="A377" s="4"/>
       <c r="B377" s="7"/>
       <c r="C377" s="7"/>
       <c r="D377" s="7"/>
       <c r="E377" s="4"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A378" s="7"/>
+    <row r="378" spans="1:5">
+      <c r="A378" s="4"/>
       <c r="B378" s="7"/>
       <c r="C378" s="7"/>
       <c r="D378" s="7"/>
       <c r="E378" s="4"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A379" s="7"/>
+    <row r="379" spans="1:5">
+      <c r="A379" s="4"/>
       <c r="B379" s="7"/>
       <c r="C379" s="7"/>
       <c r="D379" s="7"/>
       <c r="E379" s="4"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A380" s="7"/>
+    <row r="380" spans="1:5">
+      <c r="A380" s="4"/>
       <c r="B380" s="7"/>
       <c r="C380" s="7"/>
       <c r="D380" s="7"/>
       <c r="E380" s="4"/>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A381" s="7"/>
+    <row r="381" spans="1:5">
+      <c r="A381" s="4"/>
       <c r="B381" s="7"/>
       <c r="C381" s="7"/>
       <c r="D381" s="7"/>
       <c r="E381" s="4"/>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A382" s="7"/>
+    <row r="382" spans="1:5">
+      <c r="A382" s="4"/>
       <c r="B382" s="7"/>
       <c r="C382" s="7"/>
       <c r="D382" s="7"/>
       <c r="E382" s="4"/>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A383" s="7"/>
+    <row r="383" spans="1:5">
+      <c r="A383" s="4"/>
       <c r="B383" s="7"/>
       <c r="C383" s="7"/>
       <c r="D383" s="7"/>
       <c r="E383" s="4"/>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A384" s="7"/>
+    <row r="384" spans="1:5">
+      <c r="A384" s="4"/>
       <c r="B384" s="7"/>
       <c r="C384" s="7"/>
       <c r="D384" s="7"/>
       <c r="E384" s="4"/>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A385" s="7"/>
+    <row r="385" spans="1:5">
+      <c r="A385" s="4"/>
       <c r="B385" s="7"/>
       <c r="C385" s="7"/>
       <c r="D385" s="7"/>
       <c r="E385" s="4"/>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A386" s="7"/>
+    <row r="386" spans="1:5">
+      <c r="A386" s="4"/>
       <c r="B386" s="7"/>
       <c r="C386" s="7"/>
       <c r="D386" s="7"/>
       <c r="E386" s="4"/>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A387" s="7"/>
+    <row r="387" spans="1:5">
+      <c r="A387" s="4"/>
       <c r="B387" s="7"/>
       <c r="C387" s="7"/>
       <c r="D387" s="7"/>
       <c r="E387" s="4"/>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A388" s="7"/>
+    <row r="388" spans="1:5">
+      <c r="A388" s="4"/>
       <c r="B388" s="7"/>
       <c r="C388" s="7"/>
       <c r="D388" s="7"/>
       <c r="E388" s="4"/>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A389" s="7"/>
+    <row r="389" spans="1:5">
+      <c r="A389" s="4"/>
       <c r="B389" s="7"/>
       <c r="C389" s="7"/>
       <c r="D389" s="7"/>
       <c r="E389" s="4"/>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A390" s="7"/>
+    <row r="390" spans="1:5">
+      <c r="A390" s="4"/>
       <c r="B390" s="7"/>
       <c r="C390" s="7"/>
       <c r="D390" s="7"/>
       <c r="E390" s="4"/>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A391" s="7"/>
+    <row r="391" spans="1:5">
+      <c r="A391" s="4"/>
       <c r="B391" s="7"/>
       <c r="C391" s="7"/>
       <c r="D391" s="7"/>
       <c r="E391" s="4"/>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A392" s="7"/>
+    <row r="392" spans="1:5">
+      <c r="A392" s="4"/>
       <c r="B392" s="7"/>
       <c r="C392" s="7"/>
       <c r="D392" s="7"/>
       <c r="E392" s="4"/>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A393" s="7"/>
+    <row r="393" spans="1:5">
+      <c r="A393" s="4"/>
       <c r="B393" s="7"/>
       <c r="C393" s="7"/>
       <c r="D393" s="7"/>
       <c r="E393" s="4"/>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A394" s="7"/>
+    <row r="394" spans="1:5">
+      <c r="A394" s="4"/>
       <c r="B394" s="7"/>
       <c r="C394" s="7"/>
       <c r="D394" s="7"/>
       <c r="E394" s="4"/>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A395" s="7"/>
+    <row r="395" spans="1:5">
+      <c r="A395" s="4"/>
       <c r="B395" s="7"/>
       <c r="C395" s="7"/>
       <c r="D395" s="7"/>
       <c r="E395" s="4"/>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A396" s="7"/>
+    <row r="396" spans="1:5">
+      <c r="A396" s="4"/>
       <c r="B396" s="7"/>
       <c r="C396" s="7"/>
       <c r="D396" s="7"/>
       <c r="E396" s="4"/>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A397" s="7"/>
+    <row r="397" spans="1:5">
+      <c r="A397" s="4"/>
       <c r="B397" s="7"/>
       <c r="C397" s="7"/>
       <c r="D397" s="7"/>
       <c r="E397" s="4"/>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A398" s="7"/>
+    <row r="398" spans="1:5">
+      <c r="A398" s="4"/>
       <c r="B398" s="7"/>
       <c r="C398" s="7"/>
       <c r="D398" s="7"/>
       <c r="E398" s="4"/>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A399" s="7"/>
+    <row r="399" spans="1:5">
+      <c r="A399" s="4"/>
       <c r="B399" s="7"/>
       <c r="C399" s="7"/>
       <c r="D399" s="7"/>
       <c r="E399" s="4"/>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A400" s="7"/>
+    <row r="400" spans="1:5">
+      <c r="A400" s="4"/>
       <c r="B400" s="7"/>
       <c r="C400" s="7"/>
       <c r="D400" s="7"/>
       <c r="E400" s="4"/>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A401" s="7"/>
+    <row r="401" spans="1:5">
+      <c r="A401" s="4"/>
       <c r="B401" s="7"/>
       <c r="C401" s="7"/>
       <c r="D401" s="7"/>
       <c r="E401" s="4"/>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A402" s="7"/>
+    <row r="402" spans="1:5">
+      <c r="A402" s="4"/>
       <c r="B402" s="7"/>
       <c r="C402" s="7"/>
       <c r="D402" s="7"/>
       <c r="E402" s="4"/>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A403" s="7"/>
+    <row r="403" spans="1:5">
+      <c r="A403" s="4"/>
       <c r="B403" s="7"/>
       <c r="C403" s="7"/>
       <c r="D403" s="7"/>
       <c r="E403" s="4"/>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A404" s="7"/>
+    <row r="404" spans="1:5">
+      <c r="A404" s="4"/>
       <c r="B404" s="7"/>
       <c r="C404" s="7"/>
       <c r="D404" s="7"/>
       <c r="E404" s="4"/>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A405" s="7"/>
+    <row r="405" spans="1:5">
+      <c r="A405" s="4"/>
       <c r="B405" s="7"/>
       <c r="C405" s="7"/>
       <c r="D405" s="7"/>
       <c r="E405" s="4"/>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A406" s="7"/>
+    <row r="406" spans="1:5">
+      <c r="A406" s="4"/>
       <c r="B406" s="7"/>
       <c r="C406" s="7"/>
       <c r="D406" s="7"/>
       <c r="E406" s="4"/>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A407" s="7"/>
+    <row r="407" spans="1:5">
+      <c r="A407" s="4"/>
       <c r="B407" s="7"/>
       <c r="C407" s="7"/>
       <c r="D407" s="7"/>
       <c r="E407" s="4"/>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A408" s="7"/>
+    <row r="408" spans="1:5">
+      <c r="A408" s="4"/>
       <c r="B408" s="7"/>
       <c r="C408" s="7"/>
       <c r="D408" s="7"/>
       <c r="E408" s="4"/>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A409" s="7"/>
+    <row r="409" spans="1:5">
+      <c r="A409" s="4"/>
       <c r="B409" s="7"/>
       <c r="C409" s="7"/>
       <c r="D409" s="7"/>
       <c r="E409" s="4"/>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A410" s="7"/>
+    <row r="410" spans="1:5">
+      <c r="A410" s="4"/>
       <c r="B410" s="7"/>
       <c r="C410" s="7"/>
       <c r="D410" s="7"/>
       <c r="E410" s="4"/>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A411" s="7"/>
+    <row r="411" spans="1:5">
+      <c r="A411" s="4"/>
       <c r="B411" s="7"/>
       <c r="C411" s="7"/>
       <c r="D411" s="7"/>
       <c r="E411" s="4"/>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A412" s="7"/>
+    <row r="412" spans="1:5">
+      <c r="A412" s="4"/>
       <c r="B412" s="7"/>
       <c r="C412" s="7"/>
       <c r="D412" s="7"/>
       <c r="E412" s="4"/>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A413" s="7"/>
+    <row r="413" spans="1:5">
+      <c r="A413" s="4"/>
       <c r="B413" s="7"/>
       <c r="C413" s="7"/>
       <c r="D413" s="7"/>
       <c r="E413" s="4"/>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A414" s="7"/>
+    <row r="414" spans="1:5">
+      <c r="A414" s="4"/>
       <c r="B414" s="7"/>
       <c r="C414" s="7"/>
       <c r="D414" s="7"/>
       <c r="E414" s="4"/>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A415" s="7"/>
+    <row r="415" spans="1:5">
+      <c r="A415" s="4"/>
       <c r="B415" s="7"/>
       <c r="C415" s="7"/>
       <c r="D415" s="7"/>
       <c r="E415" s="4"/>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A416" s="7"/>
+    <row r="416" spans="1:5">
+      <c r="A416" s="4"/>
       <c r="B416" s="7"/>
       <c r="C416" s="7"/>
       <c r="D416" s="7"/>
       <c r="E416" s="4"/>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A417" s="7"/>
+    <row r="417" spans="1:5">
+      <c r="A417" s="4"/>
       <c r="B417" s="7"/>
       <c r="C417" s="7"/>
       <c r="D417" s="7"/>
       <c r="E417" s="4"/>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A418" s="7"/>
+    <row r="418" spans="1:5">
+      <c r="A418" s="4"/>
       <c r="B418" s="7"/>
       <c r="C418" s="7"/>
       <c r="D418" s="7"/>
       <c r="E418" s="4"/>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A419" s="7"/>
+    <row r="419" spans="1:5">
+      <c r="A419" s="4"/>
       <c r="B419" s="7"/>
       <c r="C419" s="7"/>
       <c r="D419" s="7"/>
       <c r="E419" s="4"/>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A420" s="7"/>
+    <row r="420" spans="1:5">
+      <c r="A420" s="4"/>
       <c r="B420" s="7"/>
       <c r="C420" s="7"/>
       <c r="D420" s="7"/>
       <c r="E420" s="4"/>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A421" s="7"/>
+    <row r="421" spans="1:5">
+      <c r="A421" s="4"/>
       <c r="B421" s="7"/>
       <c r="C421" s="7"/>
       <c r="D421" s="7"/>
       <c r="E421" s="4"/>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A422" s="7"/>
+    <row r="422" spans="1:5">
+      <c r="A422" s="4"/>
       <c r="B422" s="7"/>
       <c r="C422" s="7"/>
       <c r="D422" s="7"/>
       <c r="E422" s="4"/>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A423" s="7"/>
+    <row r="423" spans="1:5">
+      <c r="A423" s="4"/>
       <c r="B423" s="7"/>
       <c r="C423" s="7"/>
       <c r="D423" s="7"/>
       <c r="E423" s="4"/>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A424" s="7"/>
+    <row r="424" spans="1:5">
+      <c r="A424" s="4"/>
       <c r="B424" s="7"/>
       <c r="C424" s="7"/>
       <c r="D424" s="7"/>
       <c r="E424" s="4"/>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A425" s="7"/>
+    <row r="425" spans="1:5">
+      <c r="A425" s="4"/>
       <c r="B425" s="7"/>
       <c r="C425" s="7"/>
       <c r="D425" s="7"/>
       <c r="E425" s="4"/>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A426" s="7"/>
+    <row r="426" spans="1:5">
+      <c r="A426" s="4"/>
       <c r="B426" s="7"/>
       <c r="C426" s="7"/>
       <c r="D426" s="7"/>
       <c r="E426" s="4"/>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A427" s="7"/>
+    <row r="427" spans="1:5">
+      <c r="A427" s="4"/>
       <c r="B427" s="7"/>
       <c r="C427" s="7"/>
       <c r="D427" s="7"/>
       <c r="E427" s="4"/>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A428" s="7"/>
+    <row r="428" spans="1:5">
+      <c r="A428" s="4"/>
       <c r="B428" s="7"/>
       <c r="C428" s="7"/>
       <c r="D428" s="7"/>
       <c r="E428" s="4"/>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A429" s="7"/>
+    <row r="429" spans="1:5">
+      <c r="A429" s="4"/>
       <c r="B429" s="7"/>
       <c r="C429" s="7"/>
       <c r="D429" s="7"/>
       <c r="E429" s="4"/>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A430" s="7"/>
+    <row r="430" spans="1:5">
+      <c r="A430" s="4"/>
       <c r="B430" s="7"/>
       <c r="C430" s="7"/>
       <c r="D430" s="7"/>
       <c r="E430" s="4"/>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A431" s="7"/>
+    <row r="431" spans="1:5">
+      <c r="A431" s="4"/>
       <c r="B431" s="7"/>
       <c r="C431" s="7"/>
       <c r="D431" s="7"/>
       <c r="E431" s="4"/>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A432" s="7"/>
+    <row r="432" spans="1:5">
+      <c r="A432" s="4"/>
       <c r="B432" s="7"/>
       <c r="C432" s="7"/>
       <c r="D432" s="7"/>
       <c r="E432" s="4"/>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A433" s="7"/>
+    <row r="433" spans="1:5">
+      <c r="A433" s="4"/>
       <c r="B433" s="7"/>
       <c r="C433" s="7"/>
       <c r="D433" s="7"/>
       <c r="E433" s="4"/>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A434" s="7"/>
+    <row r="434" spans="1:5">
+      <c r="A434" s="4"/>
       <c r="B434" s="7"/>
       <c r="C434" s="7"/>
       <c r="D434" s="7"/>
       <c r="E434" s="4"/>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A435" s="7"/>
+    <row r="435" spans="1:5">
+      <c r="A435" s="4"/>
       <c r="B435" s="7"/>
       <c r="C435" s="7"/>
       <c r="D435" s="7"/>
       <c r="E435" s="4"/>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A436" s="7"/>
+    <row r="436" spans="1:5">
+      <c r="A436" s="4"/>
       <c r="B436" s="7"/>
       <c r="C436" s="7"/>
       <c r="D436" s="7"/>
       <c r="E436" s="4"/>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A437" s="7"/>
+    <row r="437" spans="1:5">
+      <c r="A437" s="4"/>
       <c r="B437" s="7"/>
       <c r="C437" s="7"/>
       <c r="D437" s="7"/>
       <c r="E437" s="4"/>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A438" s="7"/>
+    <row r="438" spans="1:5">
+      <c r="A438" s="4"/>
       <c r="B438" s="7"/>
       <c r="C438" s="7"/>
       <c r="D438" s="7"/>
       <c r="E438" s="4"/>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A439" s="7"/>
+    <row r="439" spans="1:5">
+      <c r="A439" s="4"/>
       <c r="B439" s="7"/>
       <c r="C439" s="7"/>
       <c r="D439" s="7"/>
       <c r="E439" s="4"/>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A440" s="7"/>
+    <row r="440" spans="1:5">
+      <c r="A440" s="4"/>
       <c r="B440" s="7"/>
       <c r="C440" s="7"/>
       <c r="D440" s="7"/>
       <c r="E440" s="4"/>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A441" s="7"/>
+    <row r="441" spans="1:5">
+      <c r="A441" s="4"/>
       <c r="B441" s="7"/>
       <c r="C441" s="7"/>
       <c r="D441" s="7"/>
       <c r="E441" s="4"/>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A442" s="7"/>
+    <row r="442" spans="1:5">
+      <c r="A442" s="4"/>
       <c r="B442" s="7"/>
       <c r="C442" s="7"/>
       <c r="D442" s="7"/>
       <c r="E442" s="4"/>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A443" s="7"/>
+    <row r="443" spans="1:5">
+      <c r="A443" s="4"/>
       <c r="B443" s="7"/>
       <c r="C443" s="7"/>
       <c r="D443" s="7"/>
       <c r="E443" s="4"/>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A444" s="7"/>
+    <row r="444" spans="1:5">
+      <c r="A444" s="4"/>
       <c r="B444" s="7"/>
       <c r="C444" s="7"/>
       <c r="D444" s="7"/>
       <c r="E444" s="4"/>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A445" s="7"/>
+    <row r="445" spans="1:5">
+      <c r="A445" s="4"/>
       <c r="B445" s="7"/>
       <c r="C445" s="7"/>
       <c r="D445" s="7"/>
       <c r="E445" s="4"/>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A446" s="7"/>
+    <row r="446" spans="1:5">
+      <c r="A446" s="4"/>
       <c r="B446" s="7"/>
       <c r="C446" s="7"/>
       <c r="D446" s="7"/>
       <c r="E446" s="4"/>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A447" s="7"/>
+    <row r="447" spans="1:5">
+      <c r="A447" s="4"/>
       <c r="B447" s="7"/>
       <c r="C447" s="7"/>
       <c r="D447" s="7"/>
       <c r="E447" s="4"/>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A448" s="7"/>
+    <row r="448" spans="1:5">
+      <c r="A448" s="4"/>
       <c r="B448" s="7"/>
       <c r="C448" s="7"/>
       <c r="D448" s="7"/>
       <c r="E448" s="4"/>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A449" s="7"/>
+    <row r="449" spans="1:5">
+      <c r="A449" s="4"/>
       <c r="B449" s="7"/>
       <c r="C449" s="7"/>
       <c r="D449" s="7"/>
       <c r="E449" s="4"/>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A450" s="7"/>
+    <row r="450" spans="1:5">
+      <c r="A450" s="4"/>
       <c r="B450" s="7"/>
       <c r="C450" s="7"/>
       <c r="D450" s="7"/>
       <c r="E450" s="4"/>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A451" s="7"/>
+    <row r="451" spans="1:5">
+      <c r="A451" s="4"/>
       <c r="B451" s="7"/>
       <c r="C451" s="7"/>
       <c r="D451" s="7"/>
       <c r="E451" s="4"/>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A452" s="7"/>
+    <row r="452" spans="1:5">
+      <c r="A452" s="4"/>
       <c r="B452" s="7"/>
       <c r="C452" s="7"/>
       <c r="D452" s="7"/>
       <c r="E452" s="4"/>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A453" s="7"/>
+    <row r="453" spans="1:5">
+      <c r="A453" s="4"/>
       <c r="B453" s="7"/>
       <c r="C453" s="7"/>
       <c r="D453" s="7"/>
       <c r="E453" s="4"/>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A454" s="7"/>
+    <row r="454" spans="1:5">
+      <c r="A454" s="4"/>
       <c r="B454" s="7"/>
       <c r="C454" s="7"/>
       <c r="D454" s="7"/>
       <c r="E454" s="4"/>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A455" s="7"/>
+    <row r="455" spans="1:5">
+      <c r="A455" s="4"/>
       <c r="B455" s="7"/>
       <c r="C455" s="7"/>
       <c r="D455" s="7"/>
       <c r="E455" s="4"/>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A456" s="7"/>
+    <row r="456" spans="1:5">
+      <c r="A456" s="4"/>
       <c r="B456" s="7"/>
       <c r="C456" s="7"/>
       <c r="D456" s="7"/>
       <c r="E456" s="4"/>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A457" s="7"/>
+    <row r="457" spans="1:5">
+      <c r="A457" s="4"/>
       <c r="B457" s="7"/>
       <c r="C457" s="7"/>
       <c r="D457" s="7"/>
       <c r="E457" s="4"/>
     </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A458" s="7"/>
+    <row r="458" spans="1:5">
+      <c r="A458" s="4"/>
       <c r="B458" s="7"/>
       <c r="C458" s="7"/>
       <c r="D458" s="7"/>
       <c r="E458" s="4"/>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A459" s="7"/>
+    <row r="459" spans="1:5">
+      <c r="A459" s="4"/>
       <c r="B459" s="7"/>
       <c r="C459" s="7"/>
       <c r="D459" s="7"/>
       <c r="E459" s="4"/>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A460" s="7"/>
+    <row r="460" spans="1:5">
+      <c r="A460" s="4"/>
       <c r="B460" s="7"/>
       <c r="C460" s="7"/>
       <c r="D460" s="7"/>
       <c r="E460" s="4"/>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A461" s="7"/>
+    <row r="461" spans="1:5">
+      <c r="A461" s="4"/>
       <c r="B461" s="7"/>
       <c r="C461" s="7"/>
       <c r="D461" s="7"/>
       <c r="E461" s="4"/>
     </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A462" s="7"/>
+    <row r="462" spans="1:5">
+      <c r="A462" s="4"/>
       <c r="B462" s="7"/>
       <c r="C462" s="7"/>
       <c r="D462" s="7"/>
       <c r="E462" s="4"/>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A463" s="7"/>
+    <row r="463" spans="1:5">
+      <c r="A463" s="4"/>
       <c r="B463" s="7"/>
       <c r="C463" s="7"/>
       <c r="D463" s="7"/>
       <c r="E463" s="4"/>
     </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A464" s="7"/>
+    <row r="464" spans="1:5">
+      <c r="A464" s="4"/>
       <c r="B464" s="7"/>
       <c r="C464" s="7"/>
       <c r="D464" s="7"/>
       <c r="E464" s="4"/>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A465" s="7"/>
+    <row r="465" spans="1:5">
+      <c r="A465" s="4"/>
       <c r="B465" s="7"/>
       <c r="C465" s="7"/>
       <c r="D465" s="7"/>
       <c r="E465" s="4"/>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A466" s="7"/>
+    <row r="466" spans="1:5">
+      <c r="A466" s="4"/>
       <c r="B466" s="7"/>
       <c r="C466" s="7"/>
       <c r="D466" s="7"/>
       <c r="E466" s="4"/>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A467" s="7"/>
+    <row r="467" spans="1:5">
+      <c r="A467" s="4"/>
       <c r="B467" s="7"/>
       <c r="C467" s="7"/>
       <c r="D467" s="7"/>
       <c r="E467" s="4"/>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A468" s="7"/>
+    <row r="468" spans="1:5">
+      <c r="A468" s="4"/>
       <c r="B468" s="7"/>
       <c r="C468" s="7"/>
       <c r="D468" s="7"/>
       <c r="E468" s="4"/>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A469" s="7"/>
+    <row r="469" spans="1:5">
+      <c r="A469" s="4"/>
       <c r="B469" s="7"/>
       <c r="C469" s="7"/>
       <c r="D469" s="7"/>
       <c r="E469" s="4"/>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A470" s="7"/>
+    <row r="470" spans="1:5">
+      <c r="A470" s="4"/>
       <c r="B470" s="7"/>
       <c r="C470" s="7"/>
       <c r="D470" s="7"/>
       <c r="E470" s="4"/>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A471" s="7"/>
+    <row r="471" spans="1:5">
+      <c r="A471" s="4"/>
       <c r="B471" s="7"/>
       <c r="C471" s="7"/>
       <c r="D471" s="7"/>
       <c r="E471" s="4"/>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A472" s="7"/>
+    <row r="472" spans="1:5">
+      <c r="A472" s="4"/>
       <c r="B472" s="7"/>
       <c r="C472" s="7"/>
       <c r="D472" s="7"/>
       <c r="E472" s="4"/>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A473" s="7"/>
+    <row r="473" spans="1:5">
+      <c r="A473" s="4"/>
       <c r="B473" s="7"/>
       <c r="C473" s="7"/>
       <c r="D473" s="7"/>
       <c r="E473" s="4"/>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A474" s="7"/>
+    <row r="474" spans="1:5">
+      <c r="A474" s="4"/>
       <c r="B474" s="7"/>
       <c r="C474" s="7"/>
       <c r="D474" s="7"/>
       <c r="E474" s="4"/>
     </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A475" s="7"/>
+    <row r="475" spans="1:5">
+      <c r="A475" s="4"/>
       <c r="B475" s="7"/>
       <c r="C475" s="7"/>
       <c r="D475" s="7"/>
       <c r="E475" s="4"/>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A476" s="7"/>
+    <row r="476" spans="1:5">
+      <c r="A476" s="4"/>
       <c r="B476" s="7"/>
       <c r="C476" s="7"/>
       <c r="D476" s="7"/>
       <c r="E476" s="4"/>
     </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A477" s="7"/>
+    <row r="477" spans="1:5">
+      <c r="A477" s="4"/>
       <c r="B477" s="7"/>
       <c r="C477" s="7"/>
       <c r="D477" s="7"/>
       <c r="E477" s="4"/>
     </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A478" s="7"/>
+    <row r="478" spans="1:5">
+      <c r="A478" s="4"/>
       <c r="B478" s="7"/>
       <c r="C478" s="7"/>
       <c r="D478" s="7"/>
       <c r="E478" s="4"/>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A479" s="7"/>
+    <row r="479" spans="1:5">
+      <c r="A479" s="4"/>
       <c r="B479" s="7"/>
       <c r="C479" s="7"/>
       <c r="D479" s="7"/>
       <c r="E479" s="4"/>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A480" s="7"/>
+    <row r="480" spans="1:5">
+      <c r="A480" s="4"/>
       <c r="B480" s="7"/>
       <c r="C480" s="7"/>
       <c r="D480" s="7"/>
       <c r="E480" s="4"/>
     </row>
-    <row r="481" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A481" s="7"/>
+    <row r="481" spans="1:5">
+      <c r="A481" s="4"/>
       <c r="B481" s="7"/>
       <c r="C481" s="7"/>
       <c r="D481" s="7"/>
       <c r="E481" s="4"/>
     </row>
-    <row r="482" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A482" s="7"/>
+    <row r="482" spans="1:5">
+      <c r="A482" s="4"/>
       <c r="B482" s="7"/>
       <c r="C482" s="7"/>
       <c r="D482" s="7"/>
       <c r="E482" s="4"/>
     </row>
-    <row r="483" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A483" s="7"/>
+    <row r="483" spans="1:5">
+      <c r="A483" s="4"/>
       <c r="B483" s="7"/>
       <c r="C483" s="7"/>
       <c r="D483" s="7"/>
       <c r="E483" s="4"/>
     </row>
-    <row r="484" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A484" s="7"/>
+    <row r="484" spans="1:5">
+      <c r="A484" s="4"/>
       <c r="B484" s="7"/>
       <c r="C484" s="7"/>
       <c r="D484" s="7"/>
       <c r="E484" s="4"/>
     </row>
-    <row r="485" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A485" s="7"/>
+    <row r="485" spans="1:5">
+      <c r="A485" s="4"/>
       <c r="B485" s="7"/>
       <c r="C485" s="7"/>
       <c r="D485" s="7"/>
       <c r="E485" s="4"/>
     </row>
-    <row r="486" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A486" s="7"/>
+    <row r="486" spans="1:5">
+      <c r="A486" s="4"/>
       <c r="B486" s="7"/>
       <c r="C486" s="7"/>
       <c r="D486" s="7"/>
       <c r="E486" s="4"/>
     </row>
-    <row r="487" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A487" s="7"/>
+    <row r="487" spans="1:5">
+      <c r="A487" s="4"/>
       <c r="B487" s="7"/>
       <c r="C487" s="7"/>
       <c r="D487" s="7"/>
       <c r="E487" s="4"/>
     </row>
-    <row r="488" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A488" s="7"/>
+    <row r="488" spans="1:5">
+      <c r="A488" s="4"/>
       <c r="B488" s="7"/>
       <c r="C488" s="7"/>
       <c r="D488" s="7"/>
       <c r="E488" s="4"/>
     </row>
-    <row r="489" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A489" s="7"/>
+    <row r="489" spans="1:5">
+      <c r="A489" s="4"/>
       <c r="B489" s="7"/>
       <c r="C489" s="7"/>
       <c r="D489" s="7"/>
       <c r="E489" s="4"/>
     </row>
-    <row r="490" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A490" s="7"/>
+    <row r="490" spans="1:5">
+      <c r="A490" s="4"/>
       <c r="B490" s="7"/>
       <c r="C490" s="7"/>
       <c r="D490" s="7"/>
       <c r="E490" s="4"/>
     </row>
-    <row r="491" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A491" s="7"/>
+    <row r="491" spans="1:5">
+      <c r="A491" s="4"/>
       <c r="B491" s="7"/>
       <c r="C491" s="7"/>
       <c r="D491" s="7"/>
       <c r="E491" s="4"/>
     </row>
-    <row r="492" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A492" s="7"/>
+    <row r="492" spans="1:5">
+      <c r="A492" s="4"/>
       <c r="B492" s="7"/>
       <c r="C492" s="7"/>
       <c r="D492" s="7"/>
       <c r="E492" s="4"/>
     </row>
-    <row r="493" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A493" s="7"/>
+    <row r="493" spans="1:5">
+      <c r="A493" s="4"/>
       <c r="B493" s="7"/>
       <c r="C493" s="7"/>
       <c r="D493" s="7"/>
       <c r="E493" s="4"/>
     </row>
-    <row r="494" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A494" s="7"/>
+    <row r="494" spans="1:5">
+      <c r="A494" s="4"/>
       <c r="B494" s="7"/>
       <c r="C494" s="7"/>
       <c r="D494" s="7"/>
       <c r="E494" s="4"/>
     </row>
-    <row r="495" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A495" s="7"/>
+    <row r="495" spans="1:5">
+      <c r="A495" s="4"/>
       <c r="B495" s="7"/>
       <c r="C495" s="7"/>
       <c r="D495" s="7"/>
       <c r="E495" s="4"/>
     </row>
-    <row r="496" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A496" s="7"/>
+    <row r="496" spans="1:5">
+      <c r="A496" s="4"/>
       <c r="B496" s="7"/>
       <c r="C496" s="7"/>
       <c r="D496" s="7"/>
       <c r="E496" s="4"/>
     </row>
-    <row r="497" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A497" s="7"/>
+    <row r="497" spans="1:5">
+      <c r="A497" s="4"/>
       <c r="B497" s="7"/>
       <c r="C497" s="7"/>
       <c r="D497" s="7"/>
       <c r="E497" s="4"/>
     </row>
-    <row r="498" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A498" s="7"/>
+    <row r="498" spans="1:5">
+      <c r="A498" s="4"/>
       <c r="B498" s="7"/>
       <c r="C498" s="7"/>
       <c r="D498" s="7"/>
       <c r="E498" s="4"/>
     </row>
-    <row r="499" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A499" s="7"/>
+    <row r="499" spans="1:5">
+      <c r="A499" s="4"/>
       <c r="B499" s="7"/>
       <c r="C499" s="7"/>
       <c r="D499" s="7"/>
       <c r="E499" s="4"/>
     </row>
-    <row r="500" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A500" s="7"/>
+    <row r="500" spans="1:5">
+      <c r="A500" s="4"/>
       <c r="B500" s="7"/>
       <c r="C500" s="7"/>
       <c r="D500" s="7"/>
@@ -4003,14 +4012,14 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4018,251 +4027,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100505376291F6FC345B254CE62B25F476D" ma:contentTypeVersion="10" ma:contentTypeDescription="Loo uus dokument" ma:contentTypeScope="" ma:versionID="0bc7dc08f8e4db75eb503ca2824706ae">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="595e45d7-2eb9-4664-b98e-ad279a82e308" xmlns:ns3="e65950c5-8261-4459-8a02-867ddf65e5f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7c704e7dea11501c6f008f953fdfe57d" ns2:_="" ns3:_="">
-    <xsd:import namespace="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
-    <xsd:import namespace="e65950c5-8261-4459-8a02-867ddf65e5f1"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="595e45d7-2eb9-4664-b98e-ad279a82e308" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="9" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Pildisildid" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="b9506e52-7e6f-4938-8c0d-0e8b16a3f561" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="13" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="17" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e65950c5-8261-4459-8a02-867ddf65e5f1" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="10" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{f2a168f5-0a39-4c60-9222-68737c9f6dd5}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="e65950c5-8261-4459-8a02-867ddf65e5f1">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Sisutüüp"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Pealkiri"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="595e45d7-2eb9-4664-b98e-ad279a82e308">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e65950c5-8261-4459-8a02-867ddf65e5f1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BE5AF12-352F-44FD-A82B-D7F590D68278}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03C06F47-E238-44E2-ADDE-8423F682D263}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
-    <ds:schemaRef ds:uri="e65950c5-8261-4459-8a02-867ddf65e5f1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA24363E-8A41-40E0-BDD4-0B7F48E2122D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
-    <ds:schemaRef ds:uri="e65950c5-8261-4459-8a02-867ddf65e5f1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>